<commit_message>
Altered code to make it Python 3 compatible (while breaking Python 2 compatibility)
</commit_message>
<xml_diff>
--- a/Tests/Proper Excel File.xlsx
+++ b/Tests/Proper Excel File.xlsx
@@ -1,70 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12450" windowWidth="28800" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 1 (with header)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 2 (no header)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet 1 (with header)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 2 (no header)" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>Occupation</t>
-  </si>
-  <si>
-    <t>Adrianus</t>
-  </si>
-  <si>
-    <t>Kleijngeld</t>
-  </si>
-  <si>
-    <t>Test Aumation Engineer</t>
-  </si>
-  <si>
-    <t>Christian</t>
-  </si>
-  <si>
-    <t>Bos</t>
-  </si>
-  <si>
-    <t>Test Automation Consultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  First name with leading spaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Last name with whitespace surrounding it   </t>
-  </si>
-  <si>
-    <t>Michiel</t>
-  </si>
-  <si>
-    <t>Kamp</t>
-  </si>
-  <si>
-    <t>Someone</t>
-  </si>
-  <si>
-    <t>Else</t>
-  </si>
-  <si>
-    <t>Unemployed</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,52 +338,74 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="10.28515625"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="9.85546875"/>
     <col bestFit="1" customWidth="1" max="3" min="3" width="11"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
+    <row customFormat="1" r="1" s="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>First name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Last name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Occupation</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Adrianus</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Kleijngeld</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Test Aumation Engineer</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Christian</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Test Automation Consultant</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  First name with leading spaces</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Last name with whitespace surrounding it   </t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -457,32 +426,44 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="9.42578125"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Michiel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Kamp</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Test Automation Consultant</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Someone</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Else</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>